<commit_message>
Sympathetic to amazon's GPU mem limitations
</commit_message>
<xml_diff>
--- a/Cases_To_Run.xlsx
+++ b/Cases_To_Run.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stanford\Research\GitHub\BuildingLandability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D144A62-B86C-4CC5-962A-D259384F60FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ACE7FA-C983-4830-8D8F-FCF9CB806233}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{33C11DB3-D0A2-4B49-B713-306C3C5BD973}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
added gridded image plotter and some other maintanence items
</commit_message>
<xml_diff>
--- a/Cases_To_Run.xlsx
+++ b/Cases_To_Run.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stanford\Research\GitHub\BuildingLandability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\acb\GitHub\BuildingLandability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ACE7FA-C983-4830-8D8F-FCF9CB806233}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC767BF-8F31-441F-A849-DA824570FAA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{33C11DB3-D0A2-4B49-B713-306C3C5BD973}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33C11DB3-D0A2-4B49-B713-306C3C5BD973}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="62">
   <si>
     <t>Number of Layers</t>
   </si>
@@ -63,15 +65,6 @@
     <t>Loss</t>
   </si>
   <si>
-    <t>Average Training Error</t>
-  </si>
-  <si>
-    <t>Average Validation Error</t>
-  </si>
-  <si>
-    <t>IoU</t>
-  </si>
-  <si>
     <t>Batch Norm Booleans</t>
   </si>
   <si>
@@ -90,9 +83,6 @@
     <t>Neural Net Type</t>
   </si>
   <si>
-    <t>False, False</t>
-  </si>
-  <si>
     <t>Filters</t>
   </si>
   <si>
@@ -226,6 +216,9 @@
   </si>
   <si>
     <t>32, 64, 128, 256, 512</t>
+  </si>
+  <si>
+    <t>False,False</t>
   </si>
 </sst>
 </file>
@@ -583,30 +576,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8E6278-CADB-4AB3-A965-6FBD9732B897}">
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.9453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.05078125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.47265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17.89453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" customWidth="1"/>
+    <col min="14" max="15" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" customWidth="1"/>
+    <col min="18" max="18" width="19.109375" customWidth="1"/>
+    <col min="19" max="19" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -642,39 +639,31 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>9</v>
       </c>
       <c r="C2">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D2">
+        <f>0/1000</f>
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>256</v>
@@ -683,39 +672,39 @@
         <v>70</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>9</v>
       </c>
       <c r="C3">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H3">
         <v>256</v>
@@ -724,39 +713,39 @@
         <v>70</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H4">
         <v>256</v>
@@ -765,39 +754,39 @@
         <v>70</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H5">
         <v>256</v>
@@ -806,39 +795,39 @@
         <v>70</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
       <c r="C6">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H6">
         <v>256</v>
@@ -847,39 +836,39 @@
         <v>70</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H7">
         <v>256</v>
@@ -888,39 +877,39 @@
         <v>70</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" t="s">
-        <v>19</v>
-      </c>
-      <c r="P7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>9</v>
       </c>
       <c r="C8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H8">
         <v>256</v>
@@ -929,39 +918,39 @@
         <v>70</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9">
         <v>256</v>
@@ -970,39 +959,39 @@
         <v>70</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
-      </c>
-      <c r="O9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1E-3</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>19</v>
-      </c>
-      <c r="P9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>0.01</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
       </c>
       <c r="H10">
         <v>256</v>
@@ -1011,39 +1000,39 @@
         <v>70</v>
       </c>
       <c r="J10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H11">
         <v>256</v>
@@ -1052,39 +1041,39 @@
         <v>70</v>
       </c>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
-      </c>
-      <c r="O11" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>1E-3</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>9</v>
-      </c>
-      <c r="C12">
-        <v>0.01</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>25</v>
       </c>
       <c r="H12">
         <v>256</v>
@@ -1093,39 +1082,39 @@
         <v>70</v>
       </c>
       <c r="J12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>61</v>
+      </c>
+      <c r="M12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>9</v>
       </c>
       <c r="C13">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H13">
         <v>256</v>
@@ -1134,39 +1123,39 @@
         <v>70</v>
       </c>
       <c r="J13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K13" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H14">
         <v>256</v>
@@ -1175,39 +1164,39 @@
         <v>70</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K14" t="s">
-        <v>16</v>
-      </c>
-      <c r="O14" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>9</v>
       </c>
       <c r="C15">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H15">
         <v>256</v>
@@ -1216,39 +1205,39 @@
         <v>70</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K15" t="s">
-        <v>16</v>
-      </c>
-      <c r="O15" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>9</v>
       </c>
       <c r="C16">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H16">
         <v>256</v>
@@ -1257,39 +1246,39 @@
         <v>70</v>
       </c>
       <c r="J16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O16" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
       <c r="C17">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H17">
         <v>256</v>
@@ -1298,39 +1287,39 @@
         <v>70</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O17" t="s">
-        <v>19</v>
-      </c>
-      <c r="P17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>9</v>
       </c>
       <c r="C18">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H18">
         <v>256</v>
@@ -1339,39 +1328,39 @@
         <v>70</v>
       </c>
       <c r="J18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K18" t="s">
-        <v>16</v>
-      </c>
-      <c r="O18" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>9</v>
       </c>
       <c r="C19">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H19">
         <v>256</v>
@@ -1380,39 +1369,39 @@
         <v>70</v>
       </c>
       <c r="J19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K19" t="s">
-        <v>16</v>
-      </c>
-      <c r="O19" t="s">
-        <v>19</v>
-      </c>
-      <c r="P19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H20">
         <v>256</v>
@@ -1421,39 +1410,39 @@
         <v>70</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K20" t="s">
-        <v>16</v>
-      </c>
-      <c r="O20" t="s">
-        <v>19</v>
-      </c>
-      <c r="P20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L20" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>9</v>
       </c>
       <c r="C21">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H21">
         <v>256</v>
@@ -1462,39 +1451,39 @@
         <v>70</v>
       </c>
       <c r="J21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K21" t="s">
-        <v>16</v>
-      </c>
-      <c r="O21" t="s">
-        <v>19</v>
-      </c>
-      <c r="P21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>9</v>
       </c>
       <c r="C22">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H22">
         <v>256</v>
@@ -1503,39 +1492,39 @@
         <v>70</v>
       </c>
       <c r="J22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K22" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L22" t="s">
+        <v>61</v>
+      </c>
+      <c r="M22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>9</v>
       </c>
       <c r="C23">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H23">
         <v>256</v>
@@ -1544,39 +1533,39 @@
         <v>70</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K23" t="s">
-        <v>16</v>
-      </c>
-      <c r="O23" t="s">
-        <v>19</v>
-      </c>
-      <c r="P23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L23" t="s">
+        <v>61</v>
+      </c>
+      <c r="M23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B24">
         <v>9</v>
       </c>
       <c r="C24">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H24">
         <v>256</v>
@@ -1585,39 +1574,39 @@
         <v>70</v>
       </c>
       <c r="J24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O24" t="s">
-        <v>19</v>
-      </c>
-      <c r="P24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L24" t="s">
+        <v>61</v>
+      </c>
+      <c r="M24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B25">
         <v>9</v>
       </c>
       <c r="C25">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H25">
         <v>256</v>
@@ -1626,39 +1615,39 @@
         <v>70</v>
       </c>
       <c r="J25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K25" t="s">
-        <v>16</v>
-      </c>
-      <c r="O25" t="s">
-        <v>19</v>
-      </c>
-      <c r="P25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L25" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B26">
         <v>9</v>
       </c>
       <c r="C26">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H26">
         <v>256</v>
@@ -1667,39 +1656,39 @@
         <v>70</v>
       </c>
       <c r="J26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K26" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" t="s">
-        <v>19</v>
-      </c>
-      <c r="P26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L26" t="s">
+        <v>61</v>
+      </c>
+      <c r="M26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>9</v>
       </c>
       <c r="C27">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H27">
         <v>256</v>
@@ -1708,39 +1697,39 @@
         <v>70</v>
       </c>
       <c r="J27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O27" t="s">
-        <v>19</v>
-      </c>
-      <c r="P27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L27" t="s">
+        <v>61</v>
+      </c>
+      <c r="M27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B28">
         <v>9</v>
       </c>
       <c r="C28">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H28">
         <v>256</v>
@@ -1749,39 +1738,39 @@
         <v>70</v>
       </c>
       <c r="J28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K28" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28" t="s">
-        <v>19</v>
-      </c>
-      <c r="P28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B29">
         <v>9</v>
       </c>
       <c r="C29">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H29">
         <v>256</v>
@@ -1790,39 +1779,39 @@
         <v>70</v>
       </c>
       <c r="J29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K29" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29" t="s">
-        <v>19</v>
-      </c>
-      <c r="P29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L29" t="s">
+        <v>61</v>
+      </c>
+      <c r="M29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B30">
         <v>9</v>
       </c>
       <c r="C30">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H30">
         <v>256</v>
@@ -1831,39 +1820,39 @@
         <v>70</v>
       </c>
       <c r="J30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K30" t="s">
-        <v>16</v>
-      </c>
-      <c r="O30" t="s">
-        <v>19</v>
-      </c>
-      <c r="P30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L30" t="s">
+        <v>61</v>
+      </c>
+      <c r="M30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B31">
         <v>9</v>
       </c>
       <c r="C31">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H31">
         <v>256</v>
@@ -1872,39 +1861,39 @@
         <v>70</v>
       </c>
       <c r="J31" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K31" t="s">
-        <v>16</v>
-      </c>
-      <c r="O31" t="s">
-        <v>19</v>
-      </c>
-      <c r="P31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L31" t="s">
+        <v>61</v>
+      </c>
+      <c r="M31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B32">
         <v>9</v>
       </c>
       <c r="C32">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H32">
         <v>256</v>
@@ -1913,39 +1902,40 @@
         <v>70</v>
       </c>
       <c r="J32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K32" t="s">
-        <v>16</v>
-      </c>
-      <c r="O32" t="s">
-        <v>19</v>
-      </c>
-      <c r="P32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L32" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B33">
         <v>9</v>
       </c>
       <c r="C33">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <f>2/1000</f>
+        <v>2E-3</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H33">
         <v>256</v>
@@ -1954,39 +1944,40 @@
         <v>70</v>
       </c>
       <c r="J33" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K33" t="s">
-        <v>16</v>
-      </c>
-      <c r="O33" t="s">
-        <v>19</v>
-      </c>
-      <c r="P33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L33" t="s">
+        <v>61</v>
+      </c>
+      <c r="M33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B34">
         <v>9</v>
       </c>
       <c r="C34">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <f>3/1000</f>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H34">
         <v>256</v>
@@ -1995,39 +1986,40 @@
         <v>70</v>
       </c>
       <c r="J34" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K34" t="s">
-        <v>16</v>
-      </c>
-      <c r="O34" t="s">
-        <v>19</v>
-      </c>
-      <c r="P34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L34" t="s">
+        <v>61</v>
+      </c>
+      <c r="M34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B35">
         <v>9</v>
       </c>
       <c r="C35">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <f>4/1000</f>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H35">
         <v>256</v>
@@ -2036,39 +2028,40 @@
         <v>70</v>
       </c>
       <c r="J35" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K35" t="s">
-        <v>16</v>
-      </c>
-      <c r="O35" t="s">
-        <v>19</v>
-      </c>
-      <c r="P35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L35" t="s">
+        <v>61</v>
+      </c>
+      <c r="M35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B36">
         <v>9</v>
       </c>
       <c r="C36">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <f>5/1000</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H36">
         <v>256</v>
@@ -2077,39 +2070,40 @@
         <v>70</v>
       </c>
       <c r="J36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K36" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" t="s">
-        <v>19</v>
-      </c>
-      <c r="P36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L36" t="s">
+        <v>61</v>
+      </c>
+      <c r="M36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B37">
         <v>9</v>
       </c>
       <c r="C37">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <f>6/1000</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H37">
         <v>256</v>
@@ -2118,39 +2112,40 @@
         <v>70</v>
       </c>
       <c r="J37" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K37" t="s">
-        <v>16</v>
-      </c>
-      <c r="O37" t="s">
-        <v>19</v>
-      </c>
-      <c r="P37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L37" t="s">
+        <v>61</v>
+      </c>
+      <c r="M37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B38">
         <v>9</v>
       </c>
       <c r="C38">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <f>7/1000</f>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H38">
         <v>256</v>
@@ -2159,39 +2154,40 @@
         <v>70</v>
       </c>
       <c r="J38" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" t="s">
-        <v>19</v>
-      </c>
-      <c r="P38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L38" t="s">
+        <v>61</v>
+      </c>
+      <c r="M38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B39">
         <v>9</v>
       </c>
       <c r="C39">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D39">
-        <v>8</v>
+        <f>8/1000</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H39">
         <v>256</v>
@@ -2200,39 +2196,40 @@
         <v>70</v>
       </c>
       <c r="J39" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K39" t="s">
-        <v>16</v>
-      </c>
-      <c r="O39" t="s">
-        <v>19</v>
-      </c>
-      <c r="P39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L39" t="s">
+        <v>61</v>
+      </c>
+      <c r="M39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B40">
         <v>9</v>
       </c>
       <c r="C40">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D40">
-        <v>9</v>
+        <f>9/1000</f>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H40">
         <v>256</v>
@@ -2241,39 +2238,40 @@
         <v>70</v>
       </c>
       <c r="J40" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K40" t="s">
-        <v>16</v>
-      </c>
-      <c r="O40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L40" t="s">
+        <v>61</v>
+      </c>
+      <c r="M40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B41">
         <v>9</v>
       </c>
       <c r="C41">
+        <v>1E-3</v>
+      </c>
+      <c r="D41">
+        <f>10/1000</f>
         <v>0.01</v>
       </c>
-      <c r="D41">
-        <v>10</v>
-      </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H41">
         <v>256</v>
@@ -2282,39 +2280,40 @@
         <v>70</v>
       </c>
       <c r="J41" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K41" t="s">
-        <v>16</v>
-      </c>
-      <c r="O41" t="s">
-        <v>19</v>
-      </c>
-      <c r="P41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L41" t="s">
+        <v>61</v>
+      </c>
+      <c r="M41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B42">
         <v>9</v>
       </c>
       <c r="C42">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D42">
-        <v>11</v>
+        <f>11/1000</f>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H42">
         <v>256</v>
@@ -2323,39 +2322,40 @@
         <v>70</v>
       </c>
       <c r="J42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K42" t="s">
-        <v>16</v>
-      </c>
-      <c r="O42" t="s">
-        <v>19</v>
-      </c>
-      <c r="P42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L42" t="s">
+        <v>61</v>
+      </c>
+      <c r="M42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B43">
         <v>9</v>
       </c>
       <c r="C43">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D43">
-        <v>12</v>
+        <f>12/1000</f>
+        <v>1.2E-2</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H43">
         <v>256</v>
@@ -2364,39 +2364,39 @@
         <v>70</v>
       </c>
       <c r="J43" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K43" t="s">
-        <v>16</v>
-      </c>
-      <c r="O43" t="s">
-        <v>19</v>
-      </c>
-      <c r="P43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L43" t="s">
+        <v>61</v>
+      </c>
+      <c r="M43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B44">
         <v>9</v>
       </c>
       <c r="C44">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H44">
         <v>512</v>
@@ -2405,39 +2405,39 @@
         <v>70</v>
       </c>
       <c r="J44" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K44" t="s">
-        <v>16</v>
-      </c>
-      <c r="O44" t="s">
-        <v>19</v>
-      </c>
-      <c r="P44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L44" t="s">
+        <v>61</v>
+      </c>
+      <c r="M44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B45">
         <v>9</v>
       </c>
       <c r="C45">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H45">
         <v>512</v>
@@ -2446,39 +2446,39 @@
         <v>70</v>
       </c>
       <c r="J45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K45" t="s">
-        <v>16</v>
-      </c>
-      <c r="O45" t="s">
-        <v>19</v>
-      </c>
-      <c r="P45" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L45" t="s">
+        <v>61</v>
+      </c>
+      <c r="M45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B46">
         <v>9</v>
       </c>
       <c r="C46">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H46">
         <v>512</v>
@@ -2487,39 +2487,39 @@
         <v>70</v>
       </c>
       <c r="J46" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K46" t="s">
-        <v>16</v>
-      </c>
-      <c r="O46" t="s">
-        <v>19</v>
-      </c>
-      <c r="P46" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L46" t="s">
+        <v>61</v>
+      </c>
+      <c r="M46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B47">
         <v>9</v>
       </c>
       <c r="C47">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H47">
         <v>512</v>
@@ -2528,39 +2528,39 @@
         <v>70</v>
       </c>
       <c r="J47" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K47" t="s">
-        <v>16</v>
-      </c>
-      <c r="O47" t="s">
-        <v>19</v>
-      </c>
-      <c r="P47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L47" t="s">
+        <v>61</v>
+      </c>
+      <c r="M47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B48">
         <v>9</v>
       </c>
       <c r="C48">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H48">
         <v>512</v>
@@ -2569,39 +2569,39 @@
         <v>70</v>
       </c>
       <c r="J48" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K48" t="s">
-        <v>16</v>
-      </c>
-      <c r="O48" t="s">
-        <v>19</v>
-      </c>
-      <c r="P48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L48" t="s">
+        <v>61</v>
+      </c>
+      <c r="M48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B49">
         <v>9</v>
       </c>
       <c r="C49">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H49">
         <v>512</v>
@@ -2610,39 +2610,39 @@
         <v>70</v>
       </c>
       <c r="J49" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K49" t="s">
-        <v>16</v>
-      </c>
-      <c r="O49" t="s">
-        <v>19</v>
-      </c>
-      <c r="P49" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L49" t="s">
+        <v>61</v>
+      </c>
+      <c r="M49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B50">
         <v>9</v>
       </c>
       <c r="C50">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F50">
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H50">
         <v>512</v>
@@ -2651,39 +2651,39 @@
         <v>70</v>
       </c>
       <c r="J50" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K50" t="s">
-        <v>16</v>
-      </c>
-      <c r="O50" t="s">
-        <v>19</v>
-      </c>
-      <c r="P50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L50" t="s">
+        <v>61</v>
+      </c>
+      <c r="M50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B51">
         <v>9</v>
       </c>
       <c r="C51">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H51">
         <v>512</v>
@@ -2692,39 +2692,39 @@
         <v>70</v>
       </c>
       <c r="J51" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K51" t="s">
-        <v>16</v>
-      </c>
-      <c r="O51" t="s">
+        <v>13</v>
+      </c>
+      <c r="L51" t="s">
+        <v>61</v>
+      </c>
+      <c r="M51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <v>1E-3</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
         <v>19</v>
-      </c>
-      <c r="P51" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52">
-        <v>9</v>
-      </c>
-      <c r="C52">
-        <v>0.01</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52" t="s">
-        <v>14</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52" t="s">
-        <v>23</v>
       </c>
       <c r="H52">
         <v>512</v>
@@ -2733,39 +2733,39 @@
         <v>70</v>
       </c>
       <c r="J52" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K52" t="s">
-        <v>16</v>
-      </c>
-      <c r="O52" t="s">
-        <v>19</v>
-      </c>
-      <c r="P52" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L52" t="s">
+        <v>61</v>
+      </c>
+      <c r="M52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B53">
         <v>9</v>
       </c>
       <c r="C53">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F53">
         <v>0</v>
       </c>
       <c r="G53" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H53">
         <v>512</v>
@@ -2774,39 +2774,39 @@
         <v>70</v>
       </c>
       <c r="J53" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K53" t="s">
-        <v>16</v>
-      </c>
-      <c r="O53" t="s">
-        <v>19</v>
-      </c>
-      <c r="P53" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L53" t="s">
+        <v>61</v>
+      </c>
+      <c r="M53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B54">
         <v>9</v>
       </c>
       <c r="C54">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F54">
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H54">
         <v>512</v>
@@ -2815,39 +2815,39 @@
         <v>70</v>
       </c>
       <c r="J54" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K54" t="s">
-        <v>16</v>
-      </c>
-      <c r="O54" t="s">
-        <v>19</v>
-      </c>
-      <c r="P54" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L54" t="s">
+        <v>61</v>
+      </c>
+      <c r="M54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B55">
         <v>9</v>
       </c>
       <c r="C55">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F55">
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H55">
         <v>512</v>
@@ -2856,39 +2856,39 @@
         <v>70</v>
       </c>
       <c r="J55" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K55" t="s">
-        <v>16</v>
-      </c>
-      <c r="O55" t="s">
-        <v>19</v>
-      </c>
-      <c r="P55" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L55" t="s">
+        <v>61</v>
+      </c>
+      <c r="M55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B56">
         <v>9</v>
       </c>
       <c r="C56">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F56">
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H56">
         <v>512</v>
@@ -2897,39 +2897,39 @@
         <v>70</v>
       </c>
       <c r="J56" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K56" t="s">
-        <v>16</v>
-      </c>
-      <c r="O56" t="s">
-        <v>19</v>
-      </c>
-      <c r="P56" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L56" t="s">
+        <v>61</v>
+      </c>
+      <c r="M56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B57">
         <v>9</v>
       </c>
       <c r="C57">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H57">
         <v>512</v>
@@ -2938,39 +2938,39 @@
         <v>70</v>
       </c>
       <c r="J57" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K57" t="s">
-        <v>16</v>
-      </c>
-      <c r="O57" t="s">
-        <v>19</v>
-      </c>
-      <c r="P57" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L57" t="s">
+        <v>61</v>
+      </c>
+      <c r="M57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B58">
         <v>9</v>
       </c>
       <c r="C58">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
       <c r="G58" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H58">
         <v>512</v>
@@ -2979,39 +2979,39 @@
         <v>70</v>
       </c>
       <c r="J58" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K58" t="s">
-        <v>16</v>
-      </c>
-      <c r="O58" t="s">
-        <v>19</v>
-      </c>
-      <c r="P58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L58" t="s">
+        <v>61</v>
+      </c>
+      <c r="M58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B59">
         <v>9</v>
       </c>
       <c r="C59">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F59">
         <v>0</v>
       </c>
       <c r="G59" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H59">
         <v>512</v>
@@ -3020,39 +3020,39 @@
         <v>70</v>
       </c>
       <c r="J59" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K59" t="s">
-        <v>16</v>
-      </c>
-      <c r="O59" t="s">
-        <v>19</v>
-      </c>
-      <c r="P59" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L59" t="s">
+        <v>61</v>
+      </c>
+      <c r="M59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B60">
         <v>9</v>
       </c>
       <c r="C60">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H60">
         <v>512</v>
@@ -3061,39 +3061,39 @@
         <v>70</v>
       </c>
       <c r="J60" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K60" t="s">
-        <v>16</v>
-      </c>
-      <c r="O60" t="s">
-        <v>19</v>
-      </c>
-      <c r="P60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L60" t="s">
+        <v>61</v>
+      </c>
+      <c r="M60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B61">
         <v>9</v>
       </c>
       <c r="C61">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F61">
         <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H61">
         <v>512</v>
@@ -3102,39 +3102,39 @@
         <v>70</v>
       </c>
       <c r="J61" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K61" t="s">
-        <v>16</v>
-      </c>
-      <c r="O61" t="s">
-        <v>19</v>
-      </c>
-      <c r="P61" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L61" t="s">
+        <v>61</v>
+      </c>
+      <c r="M61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B62">
         <v>9</v>
       </c>
       <c r="C62">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H62">
         <v>512</v>
@@ -3143,39 +3143,39 @@
         <v>70</v>
       </c>
       <c r="J62" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O62" t="s">
-        <v>19</v>
-      </c>
-      <c r="P62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L62" t="s">
+        <v>61</v>
+      </c>
+      <c r="M62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B63">
         <v>9</v>
       </c>
       <c r="C63">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H63">
         <v>512</v>
@@ -3184,39 +3184,39 @@
         <v>70</v>
       </c>
       <c r="J63" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K63" t="s">
-        <v>16</v>
-      </c>
-      <c r="O63" t="s">
-        <v>19</v>
-      </c>
-      <c r="P63" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L63" t="s">
+        <v>61</v>
+      </c>
+      <c r="M63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B64">
         <v>9</v>
       </c>
       <c r="C64">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F64">
         <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H64">
         <v>512</v>
@@ -3225,39 +3225,39 @@
         <v>70</v>
       </c>
       <c r="J64" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K64" t="s">
-        <v>16</v>
-      </c>
-      <c r="O64" t="s">
-        <v>19</v>
-      </c>
-      <c r="P64" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L64" t="s">
+        <v>61</v>
+      </c>
+      <c r="M64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B65">
         <v>9</v>
       </c>
       <c r="C65">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F65">
         <v>0</v>
       </c>
       <c r="G65" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H65">
         <v>512</v>
@@ -3266,39 +3266,39 @@
         <v>70</v>
       </c>
       <c r="J65" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K65" t="s">
-        <v>16</v>
-      </c>
-      <c r="O65" t="s">
-        <v>19</v>
-      </c>
-      <c r="P65" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L65" t="s">
+        <v>61</v>
+      </c>
+      <c r="M65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B66">
         <v>9</v>
       </c>
       <c r="C66">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F66">
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H66">
         <v>512</v>
@@ -3307,39 +3307,39 @@
         <v>70</v>
       </c>
       <c r="J66" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K66" t="s">
-        <v>16</v>
-      </c>
-      <c r="O66" t="s">
-        <v>19</v>
-      </c>
-      <c r="P66" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L66" t="s">
+        <v>61</v>
+      </c>
+      <c r="M66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B67">
         <v>9</v>
       </c>
       <c r="C67">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F67">
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H67">
         <v>512</v>
@@ -3348,39 +3348,39 @@
         <v>70</v>
       </c>
       <c r="J67" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K67" t="s">
-        <v>16</v>
-      </c>
-      <c r="O67" t="s">
-        <v>19</v>
-      </c>
-      <c r="P67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L67" t="s">
+        <v>61</v>
+      </c>
+      <c r="M67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B68">
         <v>9</v>
       </c>
       <c r="C68">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D68">
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F68">
         <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H68">
         <v>512</v>
@@ -3389,39 +3389,39 @@
         <v>70</v>
       </c>
       <c r="J68" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K68" t="s">
-        <v>16</v>
-      </c>
-      <c r="O68" t="s">
-        <v>19</v>
-      </c>
-      <c r="P68" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L68" t="s">
+        <v>61</v>
+      </c>
+      <c r="M68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B69">
         <v>9</v>
       </c>
       <c r="C69">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H69">
         <v>512</v>
@@ -3430,39 +3430,39 @@
         <v>70</v>
       </c>
       <c r="J69" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K69" t="s">
-        <v>16</v>
-      </c>
-      <c r="O69" t="s">
-        <v>19</v>
-      </c>
-      <c r="P69" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L69" t="s">
+        <v>61</v>
+      </c>
+      <c r="M69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B70">
         <v>9</v>
       </c>
       <c r="C70">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H70">
         <v>512</v>
@@ -3471,39 +3471,39 @@
         <v>70</v>
       </c>
       <c r="J70" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K70" t="s">
-        <v>16</v>
-      </c>
-      <c r="O70" t="s">
-        <v>19</v>
-      </c>
-      <c r="P70" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L70" t="s">
+        <v>61</v>
+      </c>
+      <c r="M70" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B71">
         <v>9</v>
       </c>
       <c r="C71">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F71">
         <v>0</v>
       </c>
       <c r="G71" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H71">
         <v>512</v>
@@ -3512,39 +3512,39 @@
         <v>70</v>
       </c>
       <c r="J71" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K71" t="s">
-        <v>16</v>
-      </c>
-      <c r="O71" t="s">
-        <v>19</v>
-      </c>
-      <c r="P71" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L71" t="s">
+        <v>61</v>
+      </c>
+      <c r="M71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B72">
         <v>9</v>
       </c>
       <c r="C72">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F72">
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H72">
         <v>512</v>
@@ -3553,39 +3553,39 @@
         <v>70</v>
       </c>
       <c r="J72" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K72" t="s">
-        <v>16</v>
-      </c>
-      <c r="O72" t="s">
-        <v>19</v>
-      </c>
-      <c r="P72" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L72" t="s">
+        <v>61</v>
+      </c>
+      <c r="M72" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B73">
         <v>9</v>
       </c>
       <c r="C73">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H73">
         <v>512</v>
@@ -3594,39 +3594,39 @@
         <v>70</v>
       </c>
       <c r="J73" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K73" t="s">
-        <v>16</v>
-      </c>
-      <c r="O73" t="s">
-        <v>19</v>
-      </c>
-      <c r="P73" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L73" t="s">
+        <v>61</v>
+      </c>
+      <c r="M73" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B74">
         <v>9</v>
       </c>
       <c r="C74">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="E74" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F74">
         <v>0</v>
       </c>
       <c r="G74" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H74">
         <v>512</v>
@@ -3635,39 +3635,40 @@
         <v>70</v>
       </c>
       <c r="J74" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K74" t="s">
-        <v>16</v>
-      </c>
-      <c r="O74" t="s">
-        <v>19</v>
-      </c>
-      <c r="P74" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L74" t="s">
+        <v>61</v>
+      </c>
+      <c r="M74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B75">
         <v>9</v>
       </c>
       <c r="C75">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <f>2/1000</f>
+        <v>2E-3</v>
       </c>
       <c r="E75" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F75">
         <v>0</v>
       </c>
       <c r="G75" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H75">
         <v>512</v>
@@ -3676,39 +3677,40 @@
         <v>70</v>
       </c>
       <c r="J75" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K75" t="s">
-        <v>16</v>
-      </c>
-      <c r="O75" t="s">
-        <v>19</v>
-      </c>
-      <c r="P75" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L75" t="s">
+        <v>61</v>
+      </c>
+      <c r="M75" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B76">
         <v>9</v>
       </c>
       <c r="C76">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D76">
-        <v>3</v>
+        <f>3/1000</f>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E76" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H76">
         <v>512</v>
@@ -3717,39 +3719,40 @@
         <v>70</v>
       </c>
       <c r="J76" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K76" t="s">
-        <v>16</v>
-      </c>
-      <c r="O76" t="s">
-        <v>19</v>
-      </c>
-      <c r="P76" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L76" t="s">
+        <v>61</v>
+      </c>
+      <c r="M76" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B77">
         <v>9</v>
       </c>
       <c r="C77">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D77">
-        <v>4</v>
+        <f>4/1000</f>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E77" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F77">
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H77">
         <v>512</v>
@@ -3758,39 +3761,40 @@
         <v>70</v>
       </c>
       <c r="J77" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K77" t="s">
-        <v>16</v>
-      </c>
-      <c r="O77" t="s">
-        <v>19</v>
-      </c>
-      <c r="P77" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L77" t="s">
+        <v>61</v>
+      </c>
+      <c r="M77" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B78">
         <v>9</v>
       </c>
       <c r="C78">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D78">
-        <v>5</v>
+        <f>5/1000</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E78" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H78">
         <v>512</v>
@@ -3799,39 +3803,40 @@
         <v>70</v>
       </c>
       <c r="J78" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K78" t="s">
-        <v>16</v>
-      </c>
-      <c r="O78" t="s">
-        <v>19</v>
-      </c>
-      <c r="P78" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L78" t="s">
+        <v>61</v>
+      </c>
+      <c r="M78" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B79">
         <v>9</v>
       </c>
       <c r="C79">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D79">
-        <v>6</v>
+        <f>6/1000</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F79">
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H79">
         <v>512</v>
@@ -3840,39 +3845,40 @@
         <v>70</v>
       </c>
       <c r="J79" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K79" t="s">
-        <v>16</v>
-      </c>
-      <c r="O79" t="s">
-        <v>19</v>
-      </c>
-      <c r="P79" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L79" t="s">
+        <v>61</v>
+      </c>
+      <c r="M79" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B80">
         <v>9</v>
       </c>
       <c r="C80">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D80">
-        <v>7</v>
+        <f>7/1000</f>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E80" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F80">
         <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H80">
         <v>512</v>
@@ -3881,39 +3887,40 @@
         <v>70</v>
       </c>
       <c r="J80" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K80" t="s">
-        <v>16</v>
-      </c>
-      <c r="O80" t="s">
-        <v>19</v>
-      </c>
-      <c r="P80" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L80" t="s">
+        <v>61</v>
+      </c>
+      <c r="M80" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B81">
         <v>9</v>
       </c>
       <c r="C81">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D81">
-        <v>8</v>
+        <f>8/1000</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E81" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F81">
         <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H81">
         <v>512</v>
@@ -3922,39 +3929,40 @@
         <v>70</v>
       </c>
       <c r="J81" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K81" t="s">
-        <v>16</v>
-      </c>
-      <c r="O81" t="s">
-        <v>19</v>
-      </c>
-      <c r="P81" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L81" t="s">
+        <v>61</v>
+      </c>
+      <c r="M81" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B82">
         <v>9</v>
       </c>
       <c r="C82">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D82">
-        <v>9</v>
+        <f>9/1000</f>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E82" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F82">
         <v>0</v>
       </c>
       <c r="G82" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H82">
         <v>512</v>
@@ -3963,39 +3971,40 @@
         <v>70</v>
       </c>
       <c r="J82" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K82" t="s">
-        <v>16</v>
-      </c>
-      <c r="O82" t="s">
-        <v>19</v>
-      </c>
-      <c r="P82" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L82" t="s">
+        <v>61</v>
+      </c>
+      <c r="M82" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B83">
         <v>9</v>
       </c>
       <c r="C83">
+        <v>1E-3</v>
+      </c>
+      <c r="D83">
+        <f>10/1000</f>
         <v>0.01</v>
       </c>
-      <c r="D83">
-        <v>10</v>
-      </c>
       <c r="E83" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F83">
         <v>0</v>
       </c>
       <c r="G83" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H83">
         <v>512</v>
@@ -4004,39 +4013,40 @@
         <v>70</v>
       </c>
       <c r="J83" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K83" t="s">
-        <v>16</v>
-      </c>
-      <c r="O83" t="s">
-        <v>19</v>
-      </c>
-      <c r="P83" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L83" t="s">
+        <v>61</v>
+      </c>
+      <c r="M83" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B84">
         <v>9</v>
       </c>
       <c r="C84">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D84">
-        <v>11</v>
+        <f>11/1000</f>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E84" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F84">
         <v>0</v>
       </c>
       <c r="G84" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H84">
         <v>512</v>
@@ -4045,39 +4055,40 @@
         <v>70</v>
       </c>
       <c r="J84" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K84" t="s">
-        <v>16</v>
-      </c>
-      <c r="O84" t="s">
-        <v>19</v>
-      </c>
-      <c r="P84" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+      <c r="L84" t="s">
+        <v>61</v>
+      </c>
+      <c r="M84" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B85">
         <v>9</v>
       </c>
       <c r="C85">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D85">
-        <v>12</v>
+        <f>12/1000</f>
+        <v>1.2E-2</v>
       </c>
       <c r="E85" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F85">
         <v>0</v>
       </c>
       <c r="G85" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H85">
         <v>512</v>
@@ -4086,16 +4097,16 @@
         <v>70</v>
       </c>
       <c r="J85" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K85" t="s">
-        <v>16</v>
-      </c>
-      <c r="O85" t="s">
-        <v>19</v>
-      </c>
-      <c r="P85" t="s">
-        <v>64</v>
+        <v>13</v>
+      </c>
+      <c r="L85" t="s">
+        <v>61</v>
+      </c>
+      <c r="M85" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>